<commit_message>
Add more awards and memberships
</commit_message>
<xml_diff>
--- a/data/award.xlsx
+++ b/data/award.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">what</t>
   </si>
@@ -47,6 +47,30 @@
   </si>
   <si>
     <t xml:space="preserve">Sponsored by The Australian Academy of Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A. Sparks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participant in workshop on “Food System Impacts of Pests &amp; Pathogens in a Changing Climate”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aspen, Colorado, USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aspen Initiative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A. Sparks &amp; D. Adorada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Best Independent Film” Award for creation of extension articles for extensionAUS website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adelaide, South Australia, AUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extensionAUS Field Disease Community of Practice</t>
   </si>
   <si>
     <t xml:space="preserve">K. Pembleton, G. Grundy, A. Sparks</t>
@@ -162,11 +186,11 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="14.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="97.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="74.29"/>
@@ -213,7 +237,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>10</v>
@@ -221,16 +245,48 @@
       <c r="D3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>